<commit_message>
Classes 6-10 OK -- 10A had wrong period distribution; corrected
</commit_message>
<xml_diff>
--- a/Timetable-2025-04-01-SAMRATH.xlsx
+++ b/Timetable-2025-04-01-SAMRATH.xlsx
@@ -854,11 +854,11 @@
   <dimension ref="A1:M220"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.23828125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -1554,7 +1554,7 @@
           <t>ROT NSQF-CG-WL (2) MB
 ENG (3) MB
 ROT SS (4) SN
-SS (1, 4, 6) JL
+SS (1, 6) JL
 ENG (5) MB</t>
         </is>
       </c>
@@ -1570,7 +1570,8 @@
           <t>MATH (2) MK
 SS (5) JL
 MATH (3) MK
-ENG (1, 4, 6) MB</t>
+ENG (1, 4) MB
+SS (6) JL</t>
         </is>
       </c>
       <c r="H11" s="51" t="inlineStr">
@@ -1590,7 +1591,7 @@
       </c>
       <c r="J11" s="51" t="inlineStr">
         <is>
-          <t>CS: 4, ENG: 7, HI: 5, IT: 6, MATH: 6, PBI: 6, PE: 6, PLB: 6, ROT ENG: 1, ROT MATH: 1, ROT NSQF-CG-WL: 1, ROT SCI: 1, ROT SS: 1, SCI: 6, SS: 4, TOTAL: 61</t>
+          <t>CS: 4, ENG: 6, HI: 5, IT: 6, MATH: 6, PBI: 6, PE: 6, PLB: 6, ROT ENG: 1, ROT MATH: 1, ROT NSQF-CG-WL: 1, ROT SCI: 1, ROT SS: 1, SCI: 6, SS: 4, TOTAL: 60</t>
         </is>
       </c>
       <c r="K11" s="51" t="inlineStr">
@@ -2057,7 +2058,7 @@
       <c r="A18" s="49" t="n"/>
       <c r="B18" s="64" t="inlineStr">
         <is>
-          <t>Last updated on Mon Apr  7 22:15:30 2025</t>
+          <t>Last updated on Mon Apr  7 22:20:15 2025</t>
         </is>
       </c>
       <c r="C18" s="65" t="n"/>
@@ -4833,7 +4834,7 @@
       </c>
       <c r="E15" s="51" t="inlineStr">
         <is>
-          <t>10A (1, 4, 6) SS
+          <t>10A (1, 6) SS
 9C (3) ROT ENG</t>
         </is>
       </c>
@@ -4848,7 +4849,8 @@
       <c r="G15" s="51" t="inlineStr">
         <is>
           <t>6B (2-3) ENG
-10A (5) SS</t>
+10A (5) SS
+10A (6) SS</t>
         </is>
       </c>
       <c r="H15" s="51" t="inlineStr">
@@ -4923,7 +4925,7 @@
       <c r="F16" s="51" t="inlineStr"/>
       <c r="G16" s="51" t="inlineStr">
         <is>
-          <t>10A (1, 4, 6) ENG
+          <t>10A (1, 4) ENG
 10C (5) SS</t>
         </is>
       </c>
@@ -4942,7 +4944,7 @@
         </is>
       </c>
       <c r="J16" s="45" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K16" s="45" t="n">
         <v>15</v>
@@ -5782,7 +5784,7 @@
       <c r="A29" s="74" t="n"/>
       <c r="B29" s="66" t="inlineStr">
         <is>
-          <t>Last updated on Mon Apr  7 22:15:30 2025</t>
+          <t>Last updated on Mon Apr  7 22:20:15 2025</t>
         </is>
       </c>
       <c r="C29" s="52" t="n"/>

</xml_diff>